<commit_message>
Cambios en el excel de la base de datos
los status y la verga
</commit_message>
<xml_diff>
--- a/fupaDocumentos/esquema de datos.xlsx
+++ b/fupaDocumentos/esquema de datos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="61">
   <si>
     <t>Clientes</t>
   </si>
@@ -186,13 +186,19 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Char(3)</t>
-  </si>
-  <si>
     <t>Desc</t>
   </si>
   <si>
     <t>credito</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Char(10)</t>
   </si>
 </sst>
 </file>
@@ -617,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -762,6 +768,12 @@
       <c r="C7" t="s">
         <v>38</v>
       </c>
+      <c r="E7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="2:16">
       <c r="B8" s="7" t="s">
@@ -811,7 +823,7 @@
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -983,7 +995,7 @@
         <v>54</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>5</v>
@@ -1063,7 +1075,7 @@
     </row>
     <row r="24" spans="2:16">
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>45</v>
@@ -1072,7 +1084,7 @@
         <v>55</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>9</v>

</xml_diff>